<commit_message>
updated base class, fixed issues to improve generated json schema
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -34,8 +34,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="25" state="visible" r:id="rId25"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="26" state="visible" r:id="rId26"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Funder" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetBase" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="28" state="visible" r:id="rId28"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1463,7 +1462,74 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>height</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>width</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1480,31 +1546,218 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>acquisition</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>instrument</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>sample</t>
+          <t>x_min</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>x_max</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>y_min</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>organizational</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>y_max</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>unit</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>value</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>detector</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>detector_mode</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1521,285 +1774,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>height</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>width</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>x_min</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>x_max</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>y_min</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>y_max</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>unit</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>value</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>calibrated_defocus</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_magnification</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>calibrated_magnification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>holder</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>holder_cryogen</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>temperature_range</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>microscope_software</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>detector_mode</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>dose_per_movie</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>energy_filter</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>image_size</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>date_time</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>exposure_time</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>cryogen</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>frames_per_movie</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>grids_imaged</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>images_generated</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>binning_camera</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>pixel_size</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>specialist_optics</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>beamshift</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>beamtilt</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>imageshift</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>beamtiltgroups</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>gainref_flip_rotate</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>used</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>width_energy_filter</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1816,42 +1810,6 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>used</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>model</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>width</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
           <t>phaseplate</t>
         </is>
       </c>

</xml_diff>

<commit_message>
added processing to oscem_spa
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -13,28 +13,29 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSize" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2D" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantityValue" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleEnv" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecimenEnv" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Freezing" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thinning" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TomogramFeatures" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleCell" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GrowthCondition" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TiltAngle" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AcquisitionTomo" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organizational" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Funder" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptors" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleEnv" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecimenEnv" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Freezing" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thinning" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TomogramFeatures" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleCell" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GrowthCondition" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TiltAngle" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AcquisitionTomo" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organizational" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Funder" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="29" state="visible" r:id="rId29"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -458,6 +459,42 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>phaseplate</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>spherical_aberration_corrector</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>chromatic_aberration_corrector</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -483,7 +520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -514,7 +551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -545,7 +582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -601,7 +638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -642,7 +679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -693,7 +730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -754,7 +791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -800,7 +837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -841,7 +878,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -887,27 +955,83 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>media</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>growth_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>cell_cycle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>treatment</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>atmosphere_growth</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>temperature_growth</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>minimal</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>maximal</t>
         </is>
@@ -918,58 +1042,173 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>media</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>growth_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>cell_cycle</t>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tilt_axis_angle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tilt_angle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>treatment</t>
+          <t>calibrated_defocus</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>atmosphere_growth</t>
+          <t>nominal_magnification</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>temperature_growth</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>detector</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>detector_mode</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -986,264 +1225,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AC1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>tilt_axis_angle</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>tilt_angle</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
+          <t>grants</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>funder</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>work_status</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>calibrated_defocus</t>
+          <t>email</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>nominal_magnification</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>calibrated_magnification</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>holder</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>holder_cryogen</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>temperature_range</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>microscope_software</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>detector_mode</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>dose_per_movie</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>energy_filter</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>image_size</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>date_time</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>exposure_time</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>cryogen</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>frames_per_movie</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>grids_imaged</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>images_generated</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>binning_camera</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>pixel_size</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>specialist_optics</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>beamshift</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>beamtilt</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>imageshift</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>beamtiltgroups</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>gainref_flip_rotate</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grants</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>funder</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>work_status</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>work_phone</t>
         </is>
       </c>
@@ -1253,7 +1290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1329,7 +1366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1380,7 +1417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1421,7 +1458,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1607,6 +1644,37 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>descriptor_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>descriptor_thing</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:AA1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1757,7 +1825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1791,40 +1859,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>phaseplate</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>spherical_aberration_corrector</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>chromatic_aberration_corrector</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ran make all to update examples and outputs
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -9,33 +9,36 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Any" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Range" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Series" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSize" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2D" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantityValue" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptors" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleEnv" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecimenEnv" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Freezing" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thinning" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TomogramFeatures" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleCell" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GrowthCondition" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TiltAngle" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AcquisitionTomo" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organizational" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Funder" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RangeSI" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Series" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSize" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2D" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2DSI" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantityValue" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantitySI" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptors" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleEnv" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecimenEnv" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Freezing" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thinning" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TomogramFeatures" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleCell" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GrowthCondition" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TiltAngle" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AcquisitionTomo" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organizational" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Funder" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -459,6 +462,193 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>descriptor_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>descriptor_thing</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>detector</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>detector_mode</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -470,6 +660,42 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>used</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>width_energy_filter</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>phaseplate</t>
         </is>
       </c>
@@ -489,7 +715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -520,7 +746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -551,7 +777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -582,7 +808,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -638,7 +864,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -679,7 +905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -730,7 +956,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -791,7 +1048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -837,7 +1094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -878,27 +1135,129 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>growth_condition</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>specimen_env</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>freezing</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>thinning</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>tomogram_features</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>media</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>growth_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>cell_cycle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>treatment</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>atmosphere_growth</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>temperature_growth</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>minimal</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>maximal</t>
         </is>
@@ -909,7 +1268,209 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tilt_axis_angle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tilt_angle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>detector</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>detector_mode</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>grants</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>funder</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -926,361 +1487,26 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>growth_condition</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>specimen_env</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>freezing</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>first_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>work_status</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>thinning</t>
+          <t>email</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>tomogram_features</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>media</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>growth_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>cell_cycle</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>treatment</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>atmosphere_growth</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>temperature_growth</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AC1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>tilt_axis_angle</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>tilt_angle</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>calibrated_defocus</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>nominal_magnification</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>calibrated_magnification</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>holder</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>holder_cryogen</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>temperature_range</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>microscope_software</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>detector_mode</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>dose_per_movie</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>energy_filter</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>image_size</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>date_time</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>exposure_time</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>cryogen</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>frames_per_movie</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>grids_imaged</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>images_generated</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>binning_camera</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>pixel_size</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>specialist_optics</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>beamshift</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>beamtilt</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>imageshift</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>beamtiltgroups</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>gainref_flip_rotate</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grants</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>funder</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>work_status</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
           <t>work_phone</t>
         </is>
       </c>
@@ -1290,7 +1516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1366,7 +1592,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>minimal_si</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximal_si</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1417,7 +1674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1458,7 +1715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1499,7 +1756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1535,7 +1792,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1566,7 +1823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1607,7 +1864,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>x_min_si</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>x_max_si</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>y_min_si</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>y_max_si</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1638,221 +1936,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>descriptor_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>descriptor_thing</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>calibrated_defocus</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_magnification</t>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>si_value</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>si_unit</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>unit</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>calibrated_magnification</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>holder</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>holder_cryogen</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>temperature_range</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>microscope_software</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>detector_mode</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>dose_per_movie</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>energy_filter</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>image_size</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>date_time</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>exposure_time</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>cryogen</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>frames_per_movie</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>grids_imaged</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>images_generated</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>binning_camera</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>pixel_size</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>specialist_optics</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>beamshift</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>beamtilt</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>imageshift</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>beamtiltgroups</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>gainref_flip_rotate</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>used</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>model</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>width_energy_filter</t>
+          <t>value</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
made SI scicat compliant
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -1953,12 +1953,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>si_value</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>si_unit</t>
+          <t>valueSI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>unitSI</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">

</xml_diff>

<commit_message>
example version including the cryoET standard
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -1298,7 +1298,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>last_name</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1369,7 +1369,7 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>last_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
@@ -1589,12 +1589,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>height</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>width</t>
+          <t>height_im</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>width_im</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Regenerate LinkML artifacts (#28)
Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -1,42 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Any" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Range" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Series" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ImageSize" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BoundingBox2D" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantityValue" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="QuantitySI" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Descriptors" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Acquisition" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EnergyFilter" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecialistOptics" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Phaseplate" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SphericalAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ChromaticAberrationCorrector" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Instrument" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleEnv" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SpecimenEnv" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Freezing" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thinning" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TomogramFeatures" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SampleCell" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GrowthCondition" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TiltAngle" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AcquisitionTomo" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Organizational" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Person" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Author" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Grant" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Funder" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EMDatasetCell" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Any" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Range" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Series" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ImageSize" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="BoundingBox2D" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="QuantityValue" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="QuantitySI" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Descriptors" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Acquisition" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="EnergyFilter" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="SpecialistOptics" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Phaseplate" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="SphericalAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="ChromaticAberrationCorrector" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Detector" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Instrument" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Microscope" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="SampleEnv" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="SpecimenEnv" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="Freezing" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Thinning" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="TomogramFeatures" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="SampleCell" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="GrowthCondition" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="TiltAngle" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="AcquisitionTomo" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="Organizational" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="Person" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="Author" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="Grant" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Funder" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="EMDatasetCell" sheetId="32" state="visible" r:id="rId32"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -625,7 +627,48 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>mode</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>dispersion</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>collection_angle</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -669,13 +712,54 @@
           <t>cs</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>operating_mode</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>beam_convergence</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>model</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>manufacturer</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -716,7 +800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -767,7 +851,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -828,7 +943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -874,27 +989,170 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>cellular_features</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>organelles</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>main_target</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>details_tomo</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>growth_condition</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>specimen_env</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>freezing</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>thinning</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>tomogram_features</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>media</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>growth_location</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>cell_cycle</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>treatment</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>atmosphere_growth</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>temperature_growth</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>minimal</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>maximal</t>
         </is>
@@ -905,48 +1163,209 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>cellular_features</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>organelles</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>main_target</t>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AC1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tilt_axis_angle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tilt_angle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>screen_current</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>details_tomo</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>detectors</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>grants</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>authors</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>funder</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -963,433 +1382,98 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>growth_condition</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>specimen_env</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>freezing</t>
+          <t>family_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>given_name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>job_title</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>thinning</t>
+          <t>email</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>tomogram_features</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>media</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>growth_location</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>cell_cycle</t>
+          <t>telephone</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>orcid</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>country</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>role</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>treatment</t>
+          <t>name_org</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>atmosphere_growth</t>
+          <t>type_org</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>temperature_growth</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AC1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>tilt_axis_angle</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>tilt_angle</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>nominal_defocus</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>calibrated_defocus</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>nominal_magnification</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>calibrated_magnification</t>
+          <t>family_name</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>holder</t>
+          <t>given_name</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>holder_cryogen</t>
+          <t>job_title</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>temperature_range</t>
+          <t>email</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>microscope_software</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>detector_mode</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>dose_per_movie</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>energy_filter</t>
-        </is>
-      </c>
-      <c r="O1" t="inlineStr">
-        <is>
-          <t>image_size</t>
-        </is>
-      </c>
-      <c r="P1" t="inlineStr">
-        <is>
-          <t>date_time</t>
-        </is>
-      </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>exposure_time</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>cryogen</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>frames_per_movie</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>grids_imaged</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>images_generated</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>binning_camera</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>pixel_size</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>specialist_optics</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>beamshift</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>beamtilt</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>imageshift</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>beamtiltgroups</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>gainref_flip_rotate</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grants</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>authors</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>funder</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>work_status</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>work_phone</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:J1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>orcid</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>country</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>role</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name_org</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>type_org</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>first_name</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>work_status</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>work_phone</t>
+          <t>telephone</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1487,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1454,7 +1574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1495,43 +1615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1764,52 +1848,52 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>screen_current</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>nominal_defocus</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>calibrated_defocus</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>nominal_magnification</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>calibrated_magnification</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>holder</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>holder_cryogen</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>temperature_range</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>microscope_software</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>detector</t>
-        </is>
-      </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>detector_mode</t>
+          <t>detectors</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">

</xml_diff>

<commit_message>
Regenerate LinkML artifacts (#41)
Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
+++ b/project/cellular_tomo/excel/oscem_schemas_cellular_tomo.xlsx
@@ -16,29 +16,33 @@
     <sheet name="QuantitySI" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="Descriptors" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="Acquisition" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="EnergyFilter" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="SpecialistOptics" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="Phaseplate" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="SphericalAberrationCorrector" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet name="ChromaticAberrationCorrector" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="Detector" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet name="Instrument" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet name="Microscope" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet name="SampleEnv" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet name="SpecimenEnv" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet name="Freezing" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet name="Thinning" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet name="TomogramFeatures" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet name="SampleCell" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet name="GrowthCondition" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet name="TiltAngle" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet name="AcquisitionTomo" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet name="Organizational" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet name="Person" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet name="Author" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet name="Grant" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet name="Funder" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet name="EMDatasetCell" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="AcquisitionSpa" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="EnergyFilter" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="SpecialistOptics" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Phaseplate" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="SphericalAberrationCorrector" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="ChromaticAberrationCorrector" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Detector" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Instrument" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Microscope" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="SampleEnv" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet name="SpecimenEnv" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet name="Freezing" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet name="Thinning" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet name="TomogramFeatures" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet name="SampleCell" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet name="GrowthCondition" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet name="TiltAngle" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet name="AcquisitionTomo" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet name="AcquisitionSubTomo" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet name="AcquisitionEnvTomo" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet name="AcquisitionCelTomo" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet name="Organizational" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet name="Person" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet name="Author" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet name="Grant" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet name="Funder" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet name="EMDatasetCell" sheetId="36" state="visible" r:id="rId36"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -462,6 +466,167 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>technique</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>screen_current</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>detectors</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -492,7 +657,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -528,7 +693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -559,7 +724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -590,7 +755,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -621,7 +786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -662,7 +827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -728,7 +893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -759,7 +924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -800,7 +965,38 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -851,38 +1047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>minimal</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -943,7 +1108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -989,7 +1154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1030,7 +1195,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1076,7 +1241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1127,7 +1292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1163,13 +1328,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AC1"/>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1190,135 +1355,689 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>technique</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>screen_current</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>detectors</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tilt_axis_angle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tilt_angle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>technique</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>screen_current</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>nominal_defocus</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>detectors</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tilt_axis_angle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tilt_angle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>technique</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>screen_current</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>calibrated_defocus</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>nominal_magnification</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>calibrated_magnification</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>holder</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>holder_cryogen</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>temperature_range</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>microscope_software</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>detectors</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>dose_per_movie</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>energy_filter</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>image_size</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>date_time</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>exposure_time</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>cryogen</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>frames_per_movie</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>grids_imaged</t>
+        </is>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>images_generated</t>
+        </is>
+      </c>
+      <c r="W1" t="inlineStr">
+        <is>
+          <t>binning_camera</t>
+        </is>
+      </c>
+      <c r="X1" t="inlineStr">
+        <is>
+          <t>pixel_size</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>specialist_optics</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>beamshift</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>beamtilt</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
+          <t>imageshift</t>
+        </is>
+      </c>
+      <c r="AC1" t="inlineStr">
+        <is>
+          <t>beamtiltgroups</t>
+        </is>
+      </c>
+      <c r="AD1" t="inlineStr">
+        <is>
+          <t>gainref_flip_rotate</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>increment</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>maximal</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>tilt_axis_angle</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>tilt_angle</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>technique</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>screen_current</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>nominal_defocus</t>
+        </is>
+      </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>calibrated_defocus</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>nominal_magnification</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>calibrated_magnification</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>holder</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>holder_cryogen</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>temperature_range</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>microscope_software</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>detectors</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>dose_per_movie</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>energy_filter</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>image_size</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>date_time</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>exposure_time</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>cryogen</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>frames_per_movie</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>grids_imaged</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>images_generated</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>binning_camera</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>pixel_size</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>specialist_optics</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>beamshift</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>beamtilt</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>imageshift</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>beamtiltgroups</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>gainref_flip_rotate</t>
         </is>
@@ -1329,7 +2048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1365,7 +2084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1411,7 +2130,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1487,69 +2206,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>increment</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>minimal</t>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>grant_name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>start_date</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>maximal</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>grant_name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>start_date</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>end_date</t>
         </is>
       </c>
@@ -1574,7 +2257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1615,7 +2298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1837,146 +2520,151 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>technique</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>screen_current</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>nominal_defocus</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>calibrated_defocus</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>nominal_magnification</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>calibrated_magnification</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>holder</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>holder_cryogen</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>temperature_range</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>microscope_software</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>detectors</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>dose_per_movie</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>energy_filter</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>image_size</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>date_time</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>exposure_time</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>cryogen</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>frames_per_movie</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>grids_imaged</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>images_generated</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>binning_camera</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>pixel_size</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>specialist_optics</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>beamshift</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>beamtilt</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>imageshift</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>beamtiltgroups</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>gainref_flip_rotate</t>
         </is>

</xml_diff>